<commit_message>
adding home picture - voacap annotated
</commit_message>
<xml_diff>
--- a/2020-05-24/TimeTable.xlsx
+++ b/2020-05-24/TimeTable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Time UTC</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>CO</t>
+  </si>
+  <si>
+    <t>20 15</t>
   </si>
 </sst>
 </file>
@@ -198,12 +201,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -213,7 +210,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -523,108 +526,131 @@
   <dimension ref="B3:P15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="6" customWidth="1"/>
-    <col min="2" max="3" width="19" style="6" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="8.140625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="19" style="4" customWidth="1"/>
+    <col min="4" max="16" width="10.5703125" style="4" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="3" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
     </row>
     <row r="4" spans="2:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
+      <c r="D5" s="7">
+        <v>20</v>
+      </c>
+      <c r="E5" s="7">
+        <v>20</v>
+      </c>
+      <c r="F5" s="7">
+        <v>20</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="7">
+        <v>20</v>
+      </c>
+      <c r="L5" s="7">
+        <v>20</v>
+      </c>
+      <c r="M5" s="7">
+        <v>20</v>
+      </c>
+      <c r="N5" s="7">
+        <v>20</v>
+      </c>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
     </row>
     <row r="6" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="7"/>
@@ -642,10 +668,10 @@
       <c r="P6" s="7"/>
     </row>
     <row r="7" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>30</v>
       </c>
       <c r="D7" s="7"/>
@@ -663,10 +689,10 @@
       <c r="P7" s="7"/>
     </row>
     <row r="8" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>0</v>
       </c>
       <c r="D8" s="7"/>
@@ -684,10 +710,10 @@
       <c r="P8" s="7"/>
     </row>
     <row r="9" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="7"/>
@@ -705,10 +731,10 @@
       <c r="P9" s="7"/>
     </row>
     <row r="10" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>320</v>
       </c>
       <c r="D10" s="7"/>
@@ -726,10 +752,10 @@
       <c r="P10" s="7"/>
     </row>
     <row r="11" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>320</v>
       </c>
       <c r="D11" s="7"/>
@@ -747,10 +773,10 @@
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="7"/>
@@ -768,10 +794,10 @@
       <c r="P12" s="7"/>
     </row>
     <row r="13" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>240</v>
       </c>
       <c r="D13" s="7"/>
@@ -789,10 +815,10 @@
       <c r="P13" s="7"/>
     </row>
     <row r="14" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="7"/>
@@ -810,10 +836,10 @@
       <c r="P14" s="7"/>
     </row>
     <row r="15" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>30</v>
       </c>
       <c r="D15" s="7"/>

</xml_diff>